<commit_message>
Auto-print vocab answers, words.xlsx clean
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miles\Documents\GitHub\Vocab-Resource-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177414EF-A30D-4FB1-919B-9669D844E7D6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750D9075-CF16-44CD-9A6A-E74BBCB88B54}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>FIRST</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>EXAMPLE</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>t</t>
   </si>
 </sst>
 </file>
@@ -421,11 +415,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:E11"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -458,116 +452,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>